<commit_message>
removed outputs as folder because the right output folder was an hidden one. I changed the right folder from hidden to not hidden
</commit_message>
<xml_diff>
--- a/outputs/guest_demographics_report.xlsx
+++ b/outputs/guest_demographics_report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Age Group</t>
   </si>
@@ -24,7 +24,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>0-25</t>
+    <t>36-45</t>
+  </si>
+  <si>
+    <t>26-35</t>
   </si>
   <si>
     <t>Nationality</t>
@@ -33,31 +36,55 @@
     <t>Switzerland</t>
   </si>
   <si>
-    <t>Guest Name</t>
-  </si>
-  <si>
-    <t>Visits</t>
-  </si>
-  <si>
-    <t>Total Nights</t>
-  </si>
-  <si>
-    <t>Last Stay</t>
-  </si>
-  <si>
-    <t>nathan jeremy</t>
-  </si>
-  <si>
-    <t>Gastname, Anzahl Besuche, Gesamtanzahl Nächte, Letzter Aufenthalt</t>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Recurring Guests</t>
+  </si>
+  <si>
+    <t>Dies ist die Anzahl der wiederkehrenden Gäste.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -110,12 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,23 +186,29 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Age Groups'!$A$2</c:f>
+              <c:f>'Age Groups'!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0-25</c:v>
+                  <c:v>36-45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26-35</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Age Groups'!$B$2</c:f>
+              <c:f>'Age Groups'!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -260,23 +292,101 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Nationalities!$A$2</c:f>
+              <c:f>Nationalities!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>United Kingdom</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>United States</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ireland</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Poland</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Portugal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Nationalities!$B$2</c:f>
+              <c:f>Nationalities!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -664,7 +774,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -683,7 +793,15 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +812,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -702,7 +820,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -710,10 +828,114 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>12</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -724,38 +946,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2">
-        <v>51413</v>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did correction to user story data visualisation
</commit_message>
<xml_diff>
--- a/outputs/guest_demographics_report.xlsx
+++ b/outputs/guest_demographics_report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Age Group</t>
   </si>
@@ -30,6 +30,9 @@
     <t>26-35</t>
   </si>
   <si>
+    <t>0-25</t>
+  </si>
+  <si>
     <t>Nationality</t>
   </si>
   <si>
@@ -75,16 +78,46 @@
     <t>Portugal</t>
   </si>
   <si>
-    <t>Recurring Guests</t>
-  </si>
-  <si>
-    <t>Dies ist die Anzahl der wiederkehrenden Gäste.</t>
+    <t>Guest Name</t>
+  </si>
+  <si>
+    <t>Visits</t>
+  </si>
+  <si>
+    <t>Total Nights</t>
+  </si>
+  <si>
+    <t>Last Stay</t>
+  </si>
+  <si>
+    <t>Muster Max</t>
+  </si>
+  <si>
+    <t>Schmidt Anna</t>
+  </si>
+  <si>
+    <t>Müller Thomas</t>
+  </si>
+  <si>
+    <t>Weber Laura</t>
+  </si>
+  <si>
+    <t>Fischer Michael</t>
+  </si>
+  <si>
+    <t>Nathan Jeremy</t>
+  </si>
+  <si>
+    <t>Gastname, Anzahl Besuche, Gesamtanzahl Nächte, Letzter Aufenthalt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -137,11 +170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,29 +220,35 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Age Groups'!$A$2:$A$3</c:f>
+              <c:f>'Age Groups'!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>36-45</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>26-35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0-25</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Age Groups'!$B$2:$B$3</c:f>
+              <c:f>'Age Groups'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,7 +387,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
@@ -774,7 +814,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -802,6 +842,14 @@
       </c>
       <c r="B3">
         <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -820,7 +868,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -828,15 +876,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -844,7 +892,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -852,7 +900,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>18</v>
@@ -860,7 +908,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -868,7 +916,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -876,7 +924,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -884,7 +932,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>17</v>
@@ -892,7 +940,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -900,7 +948,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -908,7 +956,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -916,7 +964,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -924,7 +972,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -932,7 +980,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -946,25 +994,108 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45963</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45966</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45967</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>